<commit_message>
migrated Datasets to new structure
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/17_datasets/20230623_datasets.xlsx
+++ b/webcentral/doc/01_data/17_datasets/20230623_datasets.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="385">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">releasedPlanned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specificApplication</t>
   </si>
   <si>
     <t xml:space="preserve">Prozessorientierte Basisdaten für Umweltmanagementsysteme</t>
@@ -1495,10 +1498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1580,1718 +1583,1719 @@
       <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H38" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3314,10 +3318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:Y50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3399,1720 +3403,1715 @@
       <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added weatherdata objects to tools and datasets
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/17_datasets/20230623_datasets.xlsx
+++ b/webcentral/doc/01_data/17_datasets/20230623_datasets.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="402">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t xml:space="preserve">earthobservations/wetterdienst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Central Europe Refined analysis version 1 (CER v1)</t>
   </si>
   <si>
     <t xml:space="preserve">associatedTools
@@ -1555,10 +1558,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z51"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3381,6 +3384,11 @@
       </c>
       <c r="Z51" s="5" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3403,10 +3411,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z51"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S52" activeCellId="0" sqref="S52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3491,12 +3499,12 @@
         <v>24</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
@@ -3505,13 +3513,13 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>102</v>
@@ -3526,25 +3534,25 @@
         <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>102</v>
@@ -3556,18 +3564,18 @@
         <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -3579,7 +3587,7 @@
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>102</v>
@@ -3591,21 +3599,21 @@
         <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>49</v>
@@ -3614,7 +3622,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>51</v>
@@ -3629,18 +3637,18 @@
         <v>53</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>57</v>
@@ -3649,13 +3657,13 @@
         <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>102</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>61</v>
@@ -3664,18 +3672,18 @@
         <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>63</v>
@@ -3684,7 +3692,7 @@
         <v>64</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>102</v>
@@ -3699,30 +3707,30 @@
         <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>52</v>
@@ -3734,18 +3742,18 @@
         <v>37</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>57</v>
@@ -3754,13 +3762,13 @@
         <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>102</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>61</v>
@@ -3769,12 +3777,12 @@
         <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>75</v>
@@ -3787,7 +3795,7 @@
         <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -3799,30 +3807,30 @@
         <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>83</v>
@@ -3837,12 +3845,12 @@
         <v>170</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>27</v>
@@ -3851,7 +3859,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>87</v>
@@ -3869,21 +3877,21 @@
         <v>32</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>91</v>
@@ -3892,13 +3900,13 @@
         <v>92</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>61</v>
@@ -3907,18 +3915,18 @@
         <v>37</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>96</v>
@@ -3927,13 +3935,13 @@
         <v>97</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>61</v>
@@ -3942,18 +3950,18 @@
         <v>37</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>100</v>
@@ -3962,7 +3970,7 @@
         <v>101</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>102</v>
@@ -3977,27 +3985,27 @@
         <v>37</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>107</v>
@@ -4009,30 +4017,30 @@
         <v>61</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>102</v>
@@ -4047,18 +4055,18 @@
         <v>37</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>118</v>
@@ -4067,10 +4075,10 @@
         <v>119</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>121</v>
@@ -4082,18 +4090,18 @@
         <v>37</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>123</v>
@@ -4102,7 +4110,7 @@
         <v>124</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>125</v>
@@ -4114,30 +4122,30 @@
         <v>32</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>128</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>102</v>
@@ -4152,27 +4160,27 @@
         <v>37</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>132</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>107</v>
@@ -4187,27 +4195,27 @@
         <v>37</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>107</v>
@@ -4222,18 +4230,18 @@
         <v>138</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>140</v>
@@ -4242,7 +4250,7 @@
         <v>141</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>142</v>
@@ -4257,18 +4265,18 @@
         <v>37</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>145</v>
@@ -4289,21 +4297,21 @@
         <v>32</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>149</v>
@@ -4312,7 +4320,7 @@
         <v>150</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>142</v>
@@ -4324,21 +4332,21 @@
         <v>32</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>91</v>
@@ -4347,13 +4355,13 @@
         <v>153</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>102</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>61</v>
@@ -4362,18 +4370,18 @@
         <v>37</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>156</v>
@@ -4382,10 +4390,10 @@
         <v>157</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>159</v>
@@ -4397,30 +4405,30 @@
         <v>160</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>164</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>32</v>
@@ -4432,33 +4440,33 @@
         <v>37</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>167</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>102</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>61</v>
@@ -4467,27 +4475,27 @@
         <v>37</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>82</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>83</v>
@@ -4502,18 +4510,18 @@
         <v>170</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>174</v>
@@ -4522,10 +4530,10 @@
         <v>175</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>52</v>
@@ -4534,30 +4542,30 @@
         <v>32</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>181</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>102</v>
@@ -4572,18 +4580,18 @@
         <v>37</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>185</v>
@@ -4604,21 +4612,21 @@
         <v>32</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>190</v>
@@ -4627,7 +4635,7 @@
         <v>191</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>102</v>
@@ -4642,18 +4650,18 @@
         <v>37</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>195</v>
@@ -4662,7 +4670,7 @@
         <v>196</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>102</v>
@@ -4677,18 +4685,18 @@
         <v>37</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>200</v>
@@ -4697,7 +4705,7 @@
         <v>201</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>32</v>
@@ -4712,27 +4720,27 @@
         <v>37</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>205</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>102</v>
@@ -4747,18 +4755,18 @@
         <v>37</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>208</v>
@@ -4779,21 +4787,21 @@
         <v>32</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
@@ -4812,57 +4820,57 @@
         <v>32</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
         <v>216</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>217</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>223</v>
@@ -4880,21 +4888,21 @@
         <v>32</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>227</v>
@@ -4903,7 +4911,7 @@
         <v>228</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>217</v>
@@ -4915,21 +4923,21 @@
         <v>32</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>37</v>
@@ -4941,7 +4949,7 @@
         <v>32</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>32</v>
@@ -4950,21 +4958,21 @@
         <v>32</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>235</v>
@@ -4973,7 +4981,7 @@
         <v>236</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>102</v>
@@ -4985,21 +4993,21 @@
         <v>32</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>37</v>
@@ -5008,7 +5016,7 @@
         <v>240</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>102</v>
@@ -5023,18 +5031,18 @@
         <v>37</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>242</v>
@@ -5055,21 +5063,21 @@
         <v>32</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>247</v>
@@ -5078,7 +5086,7 @@
         <v>248</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>37</v>
@@ -5090,15 +5098,15 @@
         <v>32</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>252</v>
@@ -5107,13 +5115,13 @@
         <v>252</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>37</v>
@@ -5128,21 +5136,21 @@
         <v>255</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>258</v>
@@ -5154,27 +5162,27 @@
         <v>259</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>263</v>
@@ -5183,7 +5191,7 @@
         <v>264</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>32</v>
@@ -5198,7 +5206,7 @@
         <v>37</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5206,19 +5214,19 @@
         <v>266</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="Q51" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="R51" s="4" t="s">
         <v>271</v>
@@ -5227,7 +5235,12 @@
         <v>272</v>
       </c>
       <c r="Z51" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>